<commit_message>
add \n, time modified
</commit_message>
<xml_diff>
--- a/Chatbot4Univ-main/train_tools/qna/train_data.xlsx
+++ b/Chatbot4Univ-main/train_tools/qna/train_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emme7\Desktop\Capstone-project-Ver2\ask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kim-young-woong/Desktop/Visual/Capstone/git-dir/Capston_Front/Chatbot4Univ-main/train_tools/qna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D891797F-5053-4784-A7B5-1C1AC278472B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E199002-3CC4-2C4C-BFE6-AC5779894BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29627,20 +29627,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.3984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.19921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.19921875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -29654,7 +29654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="202.2">
+    <row r="2" spans="1:4" ht="220">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -29668,7 +29668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="220.2">
+    <row r="3" spans="1:4" ht="230">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -29682,7 +29682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="275.39999999999998">
+    <row r="4" spans="1:4" ht="286">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -29696,7 +29696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="248.4">
+    <row r="5" spans="1:4" ht="271">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -29710,7 +29710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="248.4">
+    <row r="6" spans="1:4" ht="271">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -29724,7 +29724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="248.4">
+    <row r="7" spans="1:4" ht="271">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -29738,7 +29738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="156.6">
+    <row r="8" spans="1:4" ht="162">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -29752,7 +29752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="156.6">
+    <row r="9" spans="1:4" ht="162">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -29766,7 +29766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="156.6">
+    <row r="10" spans="1:4" ht="162">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -29780,7 +29780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="87">
+    <row r="11" spans="1:4" ht="90">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -29794,7 +29794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="78">
+    <row r="12" spans="1:4" ht="85">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -29808,7 +29808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="360.6">
+    <row r="13" spans="1:4" ht="389">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -29822,7 +29822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="394.8">
+    <row r="14" spans="1:4" ht="408">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -29836,7 +29836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="394.8">
+    <row r="15" spans="1:4" ht="408">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -29850,7 +29850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="109.2">
+    <row r="16" spans="1:4" ht="119">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -29864,7 +29864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="109.2">
+    <row r="17" spans="1:4" ht="119">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -29878,7 +29878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="109.2">
+    <row r="18" spans="1:4" ht="119">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -29892,7 +29892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="62.4">
+    <row r="19" spans="1:4" ht="68">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -29906,7 +29906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="69.599999999999994">
+    <row r="20" spans="1:4" ht="72">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -29920,7 +29920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34.799999999999997">
+    <row r="21" spans="1:4" ht="54">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -29934,7 +29934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="156">
+    <row r="22" spans="1:4" ht="170">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -29948,7 +29948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="34.799999999999997">
+    <row r="23" spans="1:4" ht="36">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -29962,7 +29962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34.799999999999997">
+    <row r="24" spans="1:4" ht="36">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -29976,7 +29976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="93.6">
+    <row r="25" spans="1:4" ht="102">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -29990,7 +29990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="202.8">
+    <row r="26" spans="1:4" ht="221">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -30004,7 +30004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="202.8">
+    <row r="27" spans="1:4" ht="221">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -30018,7 +30018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="226.2">
+    <row r="28" spans="1:4" ht="234">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
@@ -30032,7 +30032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34.799999999999997">
+    <row r="29" spans="1:4" ht="36">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -30046,7 +30046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="18">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -30060,7 +30060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="18">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
@@ -30074,7 +30074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="191.4">
+    <row r="32" spans="1:4" ht="198">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -30088,7 +30088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="156">
+    <row r="33" spans="1:4" ht="170">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
@@ -30102,7 +30102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="121.8">
+    <row r="34" spans="1:4" ht="126">
       <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
@@ -30116,7 +30116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="93.6">
+    <row r="35" spans="1:4" ht="102">
       <c r="A35" s="2" t="s">
         <v>5</v>
       </c>
@@ -30130,7 +30130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="93.6">
+    <row r="36" spans="1:4" ht="102">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -30144,7 +30144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="93.6">
+    <row r="37" spans="1:4" ht="102">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
@@ -30158,7 +30158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34.799999999999997">
+    <row r="38" spans="1:4" ht="36">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
@@ -30172,7 +30172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34.799999999999997">
+    <row r="39" spans="1:4" ht="36">
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
@@ -30186,7 +30186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34.799999999999997">
+    <row r="40" spans="1:4" ht="36">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -30200,7 +30200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="52.2">
+    <row r="41" spans="1:4" ht="54">
       <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
@@ -30214,7 +30214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="52.2">
+    <row r="42" spans="1:4" ht="54">
       <c r="A42" s="2" t="s">
         <v>5</v>
       </c>
@@ -30228,7 +30228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="52.2">
+    <row r="43" spans="1:4" ht="72">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
@@ -30242,7 +30242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="52.2">
+    <row r="44" spans="1:4" ht="72">
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
@@ -30256,7 +30256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="52.2">
+    <row r="45" spans="1:4" ht="72">
       <c r="A45" s="2" t="s">
         <v>5</v>
       </c>
@@ -30270,7 +30270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="52.2">
+    <row r="46" spans="1:4" ht="72">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
@@ -30284,7 +30284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="52.2">
+    <row r="47" spans="1:4" ht="72">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -30298,7 +30298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="34.799999999999997">
+    <row r="48" spans="1:4" ht="36">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -30312,7 +30312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="191.4">
+    <row r="49" spans="1:4" ht="198">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -30326,7 +30326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="191.4">
+    <row r="50" spans="1:4" ht="198">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -30340,7 +30340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="34.799999999999997">
+    <row r="51" spans="1:4" ht="36">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
@@ -30354,7 +30354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="34.799999999999997">
+    <row r="52" spans="1:4" ht="36">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -30368,7 +30368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="34.799999999999997">
+    <row r="53" spans="1:4" ht="36">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
@@ -30382,7 +30382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="34.799999999999997">
+    <row r="54" spans="1:4" ht="36">
       <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
@@ -30396,7 +30396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="34.799999999999997">
+    <row r="55" spans="1:4" ht="36">
       <c r="A55" s="2" t="s">
         <v>5</v>
       </c>
@@ -30410,7 +30410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="243.6">
+    <row r="56" spans="1:4" ht="270">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -30424,7 +30424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="34.799999999999997">
+    <row r="57" spans="1:4" ht="36">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -30438,7 +30438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="34.799999999999997">
+    <row r="58" spans="1:4" ht="36">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -30452,7 +30452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="34.799999999999997">
+    <row r="59" spans="1:4" ht="36">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -30466,7 +30466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="104.4">
+    <row r="60" spans="1:4" ht="108">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -30480,7 +30480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="104.4">
+    <row r="61" spans="1:4" ht="108">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -30494,7 +30494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="87">
+    <row r="62" spans="1:4" ht="90">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -30508,7 +30508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="69.599999999999994">
+    <row r="63" spans="1:4" ht="72">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -30522,7 +30522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="52.2">
+    <row r="64" spans="1:4" ht="54">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -30536,7 +30536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="52.2">
+    <row r="65" spans="1:4" ht="54">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
@@ -30550,7 +30550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="34.799999999999997">
+    <row r="66" spans="1:4" ht="36">
       <c r="A66" s="2" t="s">
         <v>5</v>
       </c>
@@ -30564,7 +30564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="34.799999999999997">
+    <row r="67" spans="1:4" ht="36">
       <c r="A67" s="2" t="s">
         <v>5</v>
       </c>
@@ -30578,7 +30578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="34.799999999999997">
+    <row r="68" spans="1:4" ht="36">
       <c r="A68" s="2" t="s">
         <v>5</v>
       </c>
@@ -30592,7 +30592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="34.799999999999997">
+    <row r="69" spans="1:4" ht="36">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -30606,7 +30606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="34.799999999999997">
+    <row r="70" spans="1:4" ht="36">
       <c r="A70" s="2" t="s">
         <v>5</v>
       </c>
@@ -30620,7 +30620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="34.799999999999997">
+    <row r="71" spans="1:4" ht="36">
       <c r="A71" s="2" t="s">
         <v>5</v>
       </c>
@@ -30634,7 +30634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="34.799999999999997">
+    <row r="72" spans="1:4" ht="36">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -30648,7 +30648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="34.799999999999997">
+    <row r="73" spans="1:4" ht="36">
       <c r="A73" s="2" t="s">
         <v>5</v>
       </c>
@@ -30662,7 +30662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="34.799999999999997">
+    <row r="74" spans="1:4" ht="36">
       <c r="A74" s="2" t="s">
         <v>5</v>
       </c>
@@ -30676,7 +30676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="34.799999999999997">
+    <row r="75" spans="1:4" ht="36">
       <c r="A75" s="2" t="s">
         <v>5</v>
       </c>
@@ -30690,7 +30690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="34.799999999999997">
+    <row r="76" spans="1:4" ht="36">
       <c r="A76" s="2" t="s">
         <v>5</v>
       </c>
@@ -30704,7 +30704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="34.799999999999997">
+    <row r="77" spans="1:4" ht="36">
       <c r="A77" s="2" t="s">
         <v>5</v>
       </c>
@@ -30718,7 +30718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="34.799999999999997">
+    <row r="78" spans="1:4" ht="36">
       <c r="A78" s="2" t="s">
         <v>5</v>
       </c>
@@ -30732,7 +30732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="34.799999999999997">
+    <row r="79" spans="1:4" ht="36">
       <c r="A79" s="2" t="s">
         <v>5</v>
       </c>
@@ -30746,7 +30746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="34.799999999999997">
+    <row r="80" spans="1:4" ht="36">
       <c r="A80" s="2" t="s">
         <v>5</v>
       </c>
@@ -30760,7 +30760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="34.799999999999997">
+    <row r="81" spans="1:4" ht="36">
       <c r="A81" s="2" t="s">
         <v>5</v>
       </c>
@@ -30774,7 +30774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="34.799999999999997">
+    <row r="82" spans="1:4" ht="36">
       <c r="A82" s="2" t="s">
         <v>5</v>
       </c>
@@ -30788,7 +30788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="34.799999999999997">
+    <row r="83" spans="1:4" ht="36">
       <c r="A83" s="2" t="s">
         <v>5</v>
       </c>
@@ -30802,7 +30802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="34.799999999999997">
+    <row r="84" spans="1:4" ht="36">
       <c r="A84" s="2" t="s">
         <v>5</v>
       </c>
@@ -30816,7 +30816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="34.799999999999997">
+    <row r="85" spans="1:4" ht="36">
       <c r="A85" s="2" t="s">
         <v>5</v>
       </c>
@@ -30830,7 +30830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="34.799999999999997">
+    <row r="86" spans="1:4" ht="36">
       <c r="A86" s="2" t="s">
         <v>5</v>
       </c>
@@ -30844,7 +30844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="34.799999999999997">
+    <row r="87" spans="1:4" ht="36">
       <c r="A87" s="2" t="s">
         <v>5</v>
       </c>
@@ -30858,7 +30858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="34.799999999999997">
+    <row r="88" spans="1:4" ht="36">
       <c r="A88" s="2" t="s">
         <v>5</v>
       </c>
@@ -30872,7 +30872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="34.799999999999997">
+    <row r="89" spans="1:4" ht="36">
       <c r="A89" s="2" t="s">
         <v>5</v>
       </c>
@@ -30886,7 +30886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="34.799999999999997">
+    <row r="90" spans="1:4" ht="36">
       <c r="A90" s="2" t="s">
         <v>5</v>
       </c>
@@ -30900,7 +30900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="34.799999999999997">
+    <row r="91" spans="1:4" ht="36">
       <c r="A91" s="2" t="s">
         <v>5</v>
       </c>
@@ -30914,7 +30914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="34.799999999999997">
+    <row r="92" spans="1:4" ht="36">
       <c r="A92" s="2" t="s">
         <v>5</v>
       </c>
@@ -30928,7 +30928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="34.799999999999997">
+    <row r="93" spans="1:4" ht="36">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
@@ -30942,7 +30942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="52.2">
+    <row r="94" spans="1:4" ht="54">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -30956,7 +30956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="52.2">
+    <row r="95" spans="1:4" ht="54">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
@@ -30970,7 +30970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="69.599999999999994">
+    <row r="96" spans="1:4" ht="72">
       <c r="A96" s="2" t="s">
         <v>5</v>
       </c>
@@ -30984,7 +30984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="69.599999999999994">
+    <row r="97" spans="1:4" ht="72">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -30998,7 +30998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="34.799999999999997">
+    <row r="98" spans="1:4" ht="36">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -31012,7 +31012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="34.799999999999997">
+    <row r="99" spans="1:4" ht="36">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -31026,7 +31026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="34.799999999999997">
+    <row r="100" spans="1:4" ht="36">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -31040,7 +31040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="34.799999999999997">
+    <row r="101" spans="1:4" ht="36">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -31054,7 +31054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="34.799999999999997">
+    <row r="102" spans="1:4" ht="36">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -31068,7 +31068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="34.799999999999997">
+    <row r="103" spans="1:4" ht="36">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -31082,7 +31082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="34.799999999999997">
+    <row r="104" spans="1:4" ht="36">
       <c r="A104" s="2" t="s">
         <v>5</v>
       </c>
@@ -31096,7 +31096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="34.799999999999997">
+    <row r="105" spans="1:4" ht="36">
       <c r="A105" s="2" t="s">
         <v>5</v>
       </c>
@@ -31110,7 +31110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="34.799999999999997">
+    <row r="106" spans="1:4" ht="36">
       <c r="A106" s="2" t="s">
         <v>5</v>
       </c>
@@ -31124,7 +31124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="34.799999999999997">
+    <row r="107" spans="1:4" ht="36">
       <c r="A107" s="2" t="s">
         <v>5</v>
       </c>
@@ -31138,7 +31138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="34.799999999999997">
+    <row r="108" spans="1:4" ht="36">
       <c r="A108" s="2" t="s">
         <v>5</v>
       </c>
@@ -31152,7 +31152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="52.2">
+    <row r="109" spans="1:4" ht="54">
       <c r="A109" s="2" t="s">
         <v>5</v>
       </c>
@@ -31166,7 +31166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="52.2">
+    <row r="110" spans="1:4" ht="54">
       <c r="A110" s="2" t="s">
         <v>5</v>
       </c>
@@ -31180,7 +31180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="52.2">
+    <row r="111" spans="1:4" ht="54">
       <c r="A111" s="2" t="s">
         <v>5</v>
       </c>
@@ -31194,7 +31194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="34.799999999999997">
+    <row r="112" spans="1:4" ht="36">
       <c r="A112" s="2" t="s">
         <v>5</v>
       </c>
@@ -31208,7 +31208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="34.799999999999997">
+    <row r="113" spans="1:4" ht="36">
       <c r="A113" s="2" t="s">
         <v>5</v>
       </c>
@@ -31222,7 +31222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="34.799999999999997">
+    <row r="114" spans="1:4" ht="36">
       <c r="A114" s="2" t="s">
         <v>5</v>
       </c>
@@ -31236,7 +31236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="34.799999999999997">
+    <row r="115" spans="1:4" ht="36">
       <c r="A115" s="2" t="s">
         <v>5</v>
       </c>
@@ -31250,7 +31250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="34.799999999999997">
+    <row r="116" spans="1:4" ht="36">
       <c r="A116" s="2" t="s">
         <v>5</v>
       </c>
@@ -31264,7 +31264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="34.799999999999997">
+    <row r="117" spans="1:4" ht="36">
       <c r="A117" s="2" t="s">
         <v>5</v>
       </c>
@@ -31278,7 +31278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="69.599999999999994">
+    <row r="118" spans="1:4" ht="72">
       <c r="A118" s="2" t="s">
         <v>5</v>
       </c>
@@ -31292,7 +31292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="69.599999999999994">
+    <row r="119" spans="1:4" ht="72">
       <c r="A119" s="2" t="s">
         <v>5</v>
       </c>
@@ -31306,7 +31306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="69.599999999999994">
+    <row r="120" spans="1:4" ht="72">
       <c r="A120" s="2" t="s">
         <v>5</v>
       </c>
@@ -31320,7 +31320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="34.799999999999997">
+    <row r="121" spans="1:4" ht="36">
       <c r="A121" s="2" t="s">
         <v>5</v>
       </c>
@@ -31334,7 +31334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="34.799999999999997">
+    <row r="122" spans="1:4" ht="36">
       <c r="A122" s="2" t="s">
         <v>5</v>
       </c>
@@ -31348,7 +31348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="34.799999999999997">
+    <row r="123" spans="1:4" ht="36">
       <c r="A123" s="2" t="s">
         <v>5</v>
       </c>
@@ -31362,7 +31362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="34.799999999999997">
+    <row r="124" spans="1:4" ht="36">
       <c r="A124" s="2" t="s">
         <v>5</v>
       </c>
@@ -31376,7 +31376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="34.799999999999997">
+    <row r="125" spans="1:4" ht="36">
       <c r="A125" s="2" t="s">
         <v>5</v>
       </c>
@@ -31390,7 +31390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="34.799999999999997">
+    <row r="126" spans="1:4" ht="36">
       <c r="A126" s="2" t="s">
         <v>213</v>
       </c>
@@ -31404,7 +31404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="34.799999999999997">
+    <row r="127" spans="1:4" ht="36">
       <c r="A127" s="2" t="s">
         <v>5</v>
       </c>
@@ -31418,7 +31418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="34.799999999999997">
+    <row r="128" spans="1:4" ht="36">
       <c r="A128" s="2" t="s">
         <v>5</v>
       </c>
@@ -31432,7 +31432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="52.2">
+    <row r="129" spans="1:4" ht="54">
       <c r="A129" s="2" t="s">
         <v>5</v>
       </c>
@@ -31446,7 +31446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="52.2">
+    <row r="130" spans="1:4" ht="54">
       <c r="A130" s="2" t="s">
         <v>5</v>
       </c>
@@ -31460,7 +31460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="52.2">
+    <row r="131" spans="1:4" ht="54">
       <c r="A131" s="2" t="s">
         <v>5</v>
       </c>
@@ -31474,7 +31474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="34.799999999999997">
+    <row r="132" spans="1:4" ht="36">
       <c r="A132" s="2" t="s">
         <v>5</v>
       </c>
@@ -31488,7 +31488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="34.799999999999997">
+    <row r="133" spans="1:4" ht="36">
       <c r="A133" s="2" t="s">
         <v>5</v>
       </c>
@@ -31502,7 +31502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="52.2">
+    <row r="134" spans="1:4" ht="54">
       <c r="A134" s="2" t="s">
         <v>5</v>
       </c>
@@ -31516,7 +31516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="52.2">
+    <row r="135" spans="1:4" ht="54">
       <c r="A135" s="2" t="s">
         <v>5</v>
       </c>
@@ -31530,7 +31530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="34.799999999999997">
+    <row r="136" spans="1:4" ht="36">
       <c r="A136" s="2" t="s">
         <v>5</v>
       </c>
@@ -31544,7 +31544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="34.799999999999997">
+    <row r="137" spans="1:4" ht="36">
       <c r="A137" s="2" t="s">
         <v>5</v>
       </c>
@@ -31558,7 +31558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="34.799999999999997">
+    <row r="138" spans="1:4" ht="36">
       <c r="A138" s="2" t="s">
         <v>5</v>
       </c>
@@ -31572,7 +31572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="34.799999999999997">
+    <row r="139" spans="1:4" ht="36">
       <c r="A139" s="2" t="s">
         <v>5</v>
       </c>
@@ -31586,7 +31586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="34.799999999999997">
+    <row r="140" spans="1:4" ht="36">
       <c r="A140" s="2" t="s">
         <v>5</v>
       </c>
@@ -31600,7 +31600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="34.799999999999997">
+    <row r="141" spans="1:4" ht="36">
       <c r="A141" s="2" t="s">
         <v>5</v>
       </c>
@@ -31614,7 +31614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="34.799999999999997">
+    <row r="142" spans="1:4" ht="36">
       <c r="A142" s="2" t="s">
         <v>5</v>
       </c>
@@ -31628,7 +31628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="34.799999999999997">
+    <row r="143" spans="1:4" ht="36">
       <c r="A143" s="2" t="s">
         <v>5</v>
       </c>
@@ -31642,7 +31642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="34.799999999999997">
+    <row r="144" spans="1:4" ht="36">
       <c r="A144" s="2" t="s">
         <v>5</v>
       </c>
@@ -31656,7 +31656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="34.799999999999997">
+    <row r="145" spans="1:4" ht="36">
       <c r="A145" s="2" t="s">
         <v>5</v>
       </c>
@@ -31670,7 +31670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="69.599999999999994">
+    <row r="146" spans="1:4" ht="72">
       <c r="A146" s="2" t="s">
         <v>5</v>
       </c>
@@ -31684,7 +31684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="34.799999999999997">
+    <row r="147" spans="1:4" ht="36">
       <c r="A147" s="2" t="s">
         <v>5</v>
       </c>
@@ -31698,7 +31698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="34.799999999999997">
+    <row r="148" spans="1:4" ht="36">
       <c r="A148" s="2" t="s">
         <v>5</v>
       </c>
@@ -31712,7 +31712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="34.799999999999997">
+    <row r="149" spans="1:4" ht="36">
       <c r="A149" s="2" t="s">
         <v>5</v>
       </c>
@@ -31726,7 +31726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="34.799999999999997">
+    <row r="150" spans="1:4" ht="36">
       <c r="A150" s="2" t="s">
         <v>5</v>
       </c>
@@ -31740,7 +31740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="34.799999999999997">
+    <row r="151" spans="1:4" ht="36">
       <c r="A151" s="2" t="s">
         <v>5</v>
       </c>
@@ -31754,7 +31754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="34.799999999999997">
+    <row r="152" spans="1:4" ht="36">
       <c r="A152" s="2" t="s">
         <v>5</v>
       </c>
@@ -31768,7 +31768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="34.799999999999997">
+    <row r="153" spans="1:4" ht="36">
       <c r="A153" s="2" t="s">
         <v>5</v>
       </c>
@@ -31782,7 +31782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="34.799999999999997">
+    <row r="154" spans="1:4" ht="36">
       <c r="A154" s="2" t="s">
         <v>5</v>
       </c>
@@ -31796,7 +31796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="34.799999999999997">
+    <row r="155" spans="1:4" ht="36">
       <c r="A155" s="2" t="s">
         <v>5</v>
       </c>
@@ -31810,7 +31810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="34.799999999999997">
+    <row r="156" spans="1:4" ht="36">
       <c r="A156" s="2" t="s">
         <v>5</v>
       </c>
@@ -31838,7 +31838,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="283.8">
+    <row r="158" spans="1:4" ht="298">
       <c r="A158" s="5" t="s">
         <v>259</v>
       </c>
@@ -31852,7 +31852,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="34.799999999999997">
+    <row r="159" spans="1:4" ht="36">
       <c r="A159" s="5" t="s">
         <v>259</v>
       </c>
@@ -31866,7 +31866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="34.799999999999997">
+    <row r="160" spans="1:4" ht="36">
       <c r="A160" s="5" t="s">
         <v>259</v>
       </c>
@@ -31936,7 +31936,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="58.2">
+    <row r="165" spans="1:4" ht="72">
       <c r="A165" s="5" t="s">
         <v>259</v>
       </c>
@@ -31950,7 +31950,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="66.599999999999994">
+    <row r="166" spans="1:4" ht="70">
       <c r="A166" s="5" t="s">
         <v>259</v>
       </c>
@@ -31992,7 +31992,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="327">
+    <row r="169" spans="1:4" ht="384">
       <c r="A169" s="5" t="s">
         <v>259</v>
       </c>
@@ -32006,7 +32006,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="327">
+    <row r="170" spans="1:4" ht="384">
       <c r="A170" s="5" t="s">
         <v>259</v>
       </c>
@@ -32020,7 +32020,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="34.799999999999997">
+    <row r="171" spans="1:4" ht="36">
       <c r="A171" s="5" t="s">
         <v>259</v>
       </c>
@@ -32034,7 +32034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="72">
+    <row r="172" spans="1:4" ht="97">
       <c r="A172" s="5" t="s">
         <v>259</v>
       </c>
@@ -32046,7 +32046,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="72">
+    <row r="173" spans="1:4" ht="81">
       <c r="A173" s="5" t="s">
         <v>259</v>
       </c>
@@ -32058,7 +32058,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="84">
+    <row r="174" spans="1:4" ht="88">
       <c r="A174" s="5" t="s">
         <v>259</v>
       </c>
@@ -32072,7 +32072,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="84">
+    <row r="175" spans="1:4" ht="88">
       <c r="A175" s="5" t="s">
         <v>259</v>
       </c>
@@ -32086,7 +32086,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="84">
+    <row r="176" spans="1:4" ht="88">
       <c r="A176" s="5" t="s">
         <v>259</v>
       </c>
@@ -32100,7 +32100,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="84">
+    <row r="177" spans="1:4" ht="88">
       <c r="A177" s="5" t="s">
         <v>259</v>
       </c>
@@ -32114,7 +32114,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="57.6">
+    <row r="178" spans="1:4" ht="81">
       <c r="A178" s="5" t="s">
         <v>259</v>
       </c>
@@ -32142,7 +32142,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="282">
+    <row r="180" spans="1:4" ht="332">
       <c r="A180" s="5" t="s">
         <v>259</v>
       </c>
@@ -32170,7 +32170,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="73.2">
+    <row r="182" spans="1:4" ht="81">
       <c r="A182" s="5" t="s">
         <v>259</v>
       </c>
@@ -32184,7 +32184,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="44.4">
+    <row r="183" spans="1:4" ht="65">
       <c r="A183" s="5" t="s">
         <v>259</v>
       </c>
@@ -32198,7 +32198,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="333">
+    <row r="184" spans="1:4" ht="350">
       <c r="A184" s="5" t="s">
         <v>259</v>
       </c>
@@ -32212,7 +32212,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="333">
+    <row r="185" spans="1:4" ht="350">
       <c r="A185" s="5" t="s">
         <v>259</v>
       </c>
@@ -32226,7 +32226,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="385.2">
+    <row r="186" spans="1:4" ht="401">
       <c r="A186" s="5" t="s">
         <v>259</v>
       </c>
@@ -32240,7 +32240,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="385.2">
+    <row r="187" spans="1:4" ht="401">
       <c r="A187" s="5" t="s">
         <v>259</v>
       </c>
@@ -32254,7 +32254,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="87">
+    <row r="188" spans="1:4" ht="90">
       <c r="A188" s="5" t="s">
         <v>259</v>
       </c>
@@ -32268,7 +32268,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="87">
+    <row r="189" spans="1:4" ht="90">
       <c r="A189" s="5" t="s">
         <v>259</v>
       </c>
@@ -32282,7 +32282,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="249">
+    <row r="190" spans="1:4" ht="262">
       <c r="A190" s="5" t="s">
         <v>259</v>
       </c>
@@ -32296,7 +32296,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="249">
+    <row r="191" spans="1:4" ht="262">
       <c r="A191" s="5" t="s">
         <v>259</v>
       </c>
@@ -32310,7 +32310,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="249">
+    <row r="192" spans="1:4" ht="262">
       <c r="A192" s="5" t="s">
         <v>259</v>
       </c>
@@ -32324,7 +32324,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="30">
+    <row r="193" spans="1:4" ht="36">
       <c r="A193" s="5" t="s">
         <v>259</v>
       </c>
@@ -32338,7 +32338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="165">
+    <row r="194" spans="1:4" ht="174">
       <c r="A194" s="5" t="s">
         <v>259</v>
       </c>
@@ -32352,7 +32352,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="182.4">
+    <row r="195" spans="1:4" ht="192">
       <c r="A195" s="5" t="s">
         <v>259</v>
       </c>
@@ -32366,7 +32366,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="52.2">
+    <row r="196" spans="1:4" ht="54">
       <c r="A196" s="5" t="s">
         <v>259</v>
       </c>
@@ -32380,7 +32380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="52.2">
+    <row r="197" spans="1:4" ht="54">
       <c r="A197" s="5" t="s">
         <v>259</v>
       </c>
@@ -32394,7 +32394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="44.4">
+    <row r="198" spans="1:4" ht="49">
       <c r="A198" s="5" t="s">
         <v>259</v>
       </c>
@@ -32408,7 +32408,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="44.4">
+    <row r="199" spans="1:4" ht="49">
       <c r="A199" s="5" t="s">
         <v>259</v>
       </c>
@@ -32422,7 +32422,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="66.599999999999994">
+    <row r="200" spans="1:4" ht="70">
       <c r="A200" s="5" t="s">
         <v>259</v>
       </c>
@@ -32436,7 +32436,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="266.39999999999998">
+    <row r="201" spans="1:4" ht="298">
       <c r="A201" s="5" t="s">
         <v>259</v>
       </c>
@@ -32450,7 +32450,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="266.39999999999998">
+    <row r="202" spans="1:4" ht="298">
       <c r="A202" s="5" t="s">
         <v>259</v>
       </c>
@@ -32464,7 +32464,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="182.4">
+    <row r="203" spans="1:4" ht="192">
       <c r="A203" s="5" t="s">
         <v>259</v>
       </c>
@@ -32478,7 +32478,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="58.8">
+    <row r="204" spans="1:4" ht="81">
       <c r="A204" s="5" t="s">
         <v>259</v>
       </c>
@@ -32492,7 +32492,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="57.6">
+    <row r="205" spans="1:4" ht="81">
       <c r="A205" s="5" t="s">
         <v>259</v>
       </c>
@@ -32506,7 +32506,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="57.6">
+    <row r="206" spans="1:4" ht="81">
       <c r="A206" s="5" t="s">
         <v>259</v>
       </c>
@@ -32520,7 +32520,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="72">
+    <row r="207" spans="1:4" ht="81">
       <c r="A207" s="5" t="s">
         <v>259</v>
       </c>
@@ -32534,7 +32534,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="72">
+    <row r="208" spans="1:4" ht="80">
       <c r="A208" s="5" t="s">
         <v>259</v>
       </c>
@@ -32548,7 +32548,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="72">
+    <row r="209" spans="1:4" ht="80">
       <c r="A209" s="5" t="s">
         <v>259</v>
       </c>
@@ -32562,7 +32562,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="34.799999999999997">
+    <row r="210" spans="1:4" ht="36">
       <c r="A210" s="5" t="s">
         <v>259</v>
       </c>
@@ -32576,7 +32576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="34.799999999999997">
+    <row r="211" spans="1:4" ht="36">
       <c r="A211" s="5" t="s">
         <v>259</v>
       </c>
@@ -32590,7 +32590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="163.19999999999999">
+    <row r="212" spans="1:4" ht="177">
       <c r="A212" s="5" t="s">
         <v>259</v>
       </c>
@@ -32604,7 +32604,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="43.2">
+    <row r="213" spans="1:4" ht="49">
       <c r="A213" s="5" t="s">
         <v>259</v>
       </c>
@@ -32618,7 +32618,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="43.2">
+    <row r="214" spans="1:4" ht="49">
       <c r="A214" s="5" t="s">
         <v>259</v>
       </c>
@@ -32632,7 +32632,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="44.4">
+    <row r="215" spans="1:4" ht="65">
       <c r="A215" s="5" t="s">
         <v>259</v>
       </c>
@@ -32646,7 +32646,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="365.4">
+    <row r="216" spans="1:4" ht="377">
       <c r="A216" s="5" t="s">
         <v>259</v>
       </c>
@@ -32660,7 +32660,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="303">
+    <row r="217" spans="1:4" ht="316">
       <c r="A217" s="5" t="s">
         <v>259</v>
       </c>
@@ -32674,7 +32674,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="73.2">
+    <row r="218" spans="1:4" ht="81">
       <c r="A218" s="5" t="s">
         <v>259</v>
       </c>
@@ -32688,7 +32688,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="72">
+    <row r="219" spans="1:4" ht="81">
       <c r="A219" s="5" t="s">
         <v>259</v>
       </c>
@@ -32702,7 +32702,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="44.4">
+    <row r="220" spans="1:4" ht="49">
       <c r="A220" s="5" t="s">
         <v>259</v>
       </c>
@@ -32716,7 +32716,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="44.4">
+    <row r="221" spans="1:4" ht="49">
       <c r="A221" s="5" t="s">
         <v>259</v>
       </c>
@@ -32730,7 +32730,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="44.4">
+    <row r="222" spans="1:4" ht="65">
       <c r="A222" s="5" t="s">
         <v>259</v>
       </c>
@@ -32744,7 +32744,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="58.8">
+    <row r="223" spans="1:4" ht="81">
       <c r="A223" s="5" t="s">
         <v>259</v>
       </c>
@@ -32758,7 +32758,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="58.8">
+    <row r="224" spans="1:4" ht="81">
       <c r="A224" s="5" t="s">
         <v>259</v>
       </c>
@@ -32772,7 +32772,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="34.799999999999997">
+    <row r="225" spans="1:4" ht="36">
       <c r="A225" s="5" t="s">
         <v>259</v>
       </c>
@@ -32786,7 +32786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="34.799999999999997">
+    <row r="226" spans="1:4" ht="36">
       <c r="A226" s="5" t="s">
         <v>259</v>
       </c>
@@ -32800,7 +32800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="58.8">
+    <row r="227" spans="1:4" ht="81">
       <c r="A227" s="5" t="s">
         <v>259</v>
       </c>
@@ -32814,7 +32814,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="58.8">
+    <row r="228" spans="1:4" ht="81">
       <c r="A228" s="5" t="s">
         <v>259</v>
       </c>
@@ -32828,7 +32828,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="58.8">
+    <row r="229" spans="1:4" ht="81">
       <c r="A229" s="5" t="s">
         <v>259</v>
       </c>
@@ -32870,7 +32870,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="263.39999999999998">
+    <row r="232" spans="1:4" ht="278">
       <c r="A232" s="5" t="s">
         <v>259</v>
       </c>
@@ -32912,7 +32912,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="58.8">
+    <row r="235" spans="1:4" ht="81">
       <c r="A235" s="5" t="s">
         <v>259</v>
       </c>
@@ -32926,7 +32926,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="34.799999999999997">
+    <row r="236" spans="1:4" ht="36">
       <c r="A236" s="5" t="s">
         <v>259</v>
       </c>
@@ -32940,7 +32940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="31.2">
+    <row r="237" spans="1:4" ht="33">
       <c r="A237" s="5" t="s">
         <v>259</v>
       </c>
@@ -32954,7 +32954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="115.8">
+    <row r="238" spans="1:4" ht="122">
       <c r="A238" s="5" t="s">
         <v>259</v>
       </c>
@@ -32968,7 +32968,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="133.19999999999999">
+    <row r="239" spans="1:4" ht="140">
       <c r="A239" s="5" t="s">
         <v>259</v>
       </c>
@@ -32982,7 +32982,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="73.2">
+    <row r="240" spans="1:4" ht="81">
       <c r="A240" s="5" t="s">
         <v>259</v>
       </c>
@@ -32996,7 +32996,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="103.8">
+    <row r="241" spans="1:4" ht="122">
       <c r="A241" s="5" t="s">
         <v>259</v>
       </c>
@@ -33010,7 +33010,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="103.8">
+    <row r="242" spans="1:4" ht="122">
       <c r="A242" s="5" t="s">
         <v>259</v>
       </c>
@@ -33024,7 +33024,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="103.8">
+    <row r="243" spans="1:4" ht="122">
       <c r="A243" s="5" t="s">
         <v>259</v>
       </c>
@@ -33038,7 +33038,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="178.2">
+    <row r="244" spans="1:4" ht="193">
       <c r="A244" s="5" t="s">
         <v>259</v>
       </c>
@@ -33052,7 +33052,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="178.2">
+    <row r="245" spans="1:4" ht="192">
       <c r="A245" s="5" t="s">
         <v>259</v>
       </c>
@@ -33066,7 +33066,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="103.8">
+    <row r="246" spans="1:4" ht="112">
       <c r="A246" s="5" t="s">
         <v>259</v>
       </c>
@@ -33080,7 +33080,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="103.8">
+    <row r="247" spans="1:4" ht="112">
       <c r="A247" s="5" t="s">
         <v>259</v>
       </c>
@@ -33094,7 +33094,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="103.8">
+    <row r="248" spans="1:4" ht="112">
       <c r="A248" s="5" t="s">
         <v>259</v>
       </c>
@@ -33108,7 +33108,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="139.19999999999999">
+    <row r="249" spans="1:4" ht="144">
       <c r="A249" s="5" t="s">
         <v>259</v>
       </c>
@@ -33122,7 +33122,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="58.8">
+    <row r="250" spans="1:4" ht="81">
       <c r="A250" s="5" t="s">
         <v>259</v>
       </c>
@@ -33136,7 +33136,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="58.8">
+    <row r="251" spans="1:4" ht="81">
       <c r="A251" s="5" t="s">
         <v>259</v>
       </c>
@@ -33150,7 +33150,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="52.2">
+    <row r="252" spans="1:4" ht="54">
       <c r="A252" s="5" t="s">
         <v>259</v>
       </c>
@@ -33164,7 +33164,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="52.2">
+    <row r="253" spans="1:4" ht="54">
       <c r="A253" s="5" t="s">
         <v>259</v>
       </c>

</xml_diff>